<commit_message>
still working on final
</commit_message>
<xml_diff>
--- a/Final/FinalProject.xlsx
+++ b/Final/FinalProject.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/claytoncohn/Dropbox/New/DePaul/CSC594/Final/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{1D9D08DE-456E-4641-BEE4-8C8C6CDE53F9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{0168C5D8-69A2-DE4E-8F3A-33231FE2DE22}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="15500"/>
   </bookViews>
@@ -18,12 +18,23 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">FinalProject!$A$1:$M$1</definedName>
   </definedNames>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="79">
   <si>
     <t>datetime</t>
   </si>
@@ -212,6 +223,54 @@
   </si>
   <si>
     <t>num</t>
+  </si>
+  <si>
+    <t>All data</t>
+  </si>
+  <si>
+    <t>15+</t>
+  </si>
+  <si>
+    <t>No relation 1000</t>
+  </si>
+  <si>
+    <t>Bagging</t>
+  </si>
+  <si>
+    <t>Few-shot</t>
+  </si>
+  <si>
+    <t>Method</t>
+  </si>
+  <si>
+    <t>Acc</t>
+  </si>
+  <si>
+    <t>mac_p</t>
+  </si>
+  <si>
+    <t>mac_r</t>
+  </si>
+  <si>
+    <t>mac_f1</t>
+  </si>
+  <si>
+    <t>mic_p</t>
+  </si>
+  <si>
+    <t>mic_r</t>
+  </si>
+  <si>
+    <t>mic_f1</t>
+  </si>
+  <si>
+    <t>All</t>
+  </si>
+  <si>
+    <t>Cropped</t>
+  </si>
+  <si>
+    <t>O 1000</t>
   </si>
 </sst>
 </file>
@@ -354,7 +413,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="38">
+  <fills count="39">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -564,6 +623,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.34998626667073579"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="10">
     <border>
@@ -725,7 +790,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
@@ -735,6 +800,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="38" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -791,6 +858,1249 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>All</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>FinalProject!$C$34:$I$34</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>Acc</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>mac_p</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>mac_r</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>mac_f1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>mic_p</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>mic_r</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>mic_f1</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>FinalProject!$C$35:$I$35</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>0.70329206570861558</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.52311198274858794</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.50145421213850783</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.48680568479667824</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.7139857994580977</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.72125218942274305</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.70998326626870367</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-C9F7-C744-B139-3166B94E8946}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Cropped</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>FinalProject!$C$34:$I$34</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>Acc</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>mac_p</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>mac_r</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>mac_f1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>mic_p</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>mic_r</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>mic_f1</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>FinalProject!$C$36:$I$36</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>0.71669260590504691</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.52592620707718185</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.5017797485497717</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.49059497183297041</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.72386407535312203</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.73049347439134571</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.71817407645282905</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-C9F7-C744-B139-3166B94E8946}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>O 1000</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent3"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>FinalProject!$C$34:$I$34</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>Acc</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>mac_p</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>mac_r</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>mac_f1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>mic_p</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>mic_r</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>mic_f1</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>FinalProject!$C$37:$I$37</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>0.59204270461013797</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.57884360502790888</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.50256460083823262</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.49889148104691994</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.60898821490402066</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.60478424180737389</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.58939676514697903</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-C9F7-C744-B139-3166B94E8946}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:v>Bagging</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent4"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>FinalProject!$C$34:$I$34</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>Acc</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>mac_p</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>mac_r</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>mac_f1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>mic_p</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>mic_r</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>mic_f1</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>FinalProject!$C$38:$I$38</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>0.4538461538461534</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.5779830133634476</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.53690382081686372</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.51559002327325254</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.5779830133634476</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.53690382081686372</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.51559002327325254</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-C9F7-C744-B139-3166B94E8946}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:v>Few-shot</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent5"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>FinalProject!$C$34:$I$34</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>Acc</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>mac_p</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>mac_r</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>mac_f1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>mic_p</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>mic_r</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>mic_f1</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>FinalProject!$C$39:$I$39</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>0.42172329706607614</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.55822577659043782</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.61085775284772714</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.51773158451892021</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.59188025671325439</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.53695889623454973</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.5043924314176832</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-C9F7-C744-B139-3166B94E8946}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="1113423008"/>
+        <c:axId val="1113416016"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1113423008"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1113416016"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1113416016"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1113423008"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>203200</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>482600</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="6" name="Chart 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{84F89F7D-9594-1F4D-8CDA-D82D98D29897}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1090,10 +2400,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M26"/>
+  <dimension ref="A1:M39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1:H1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="K43" sqref="K43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1974,7 +3284,7 @@
     </row>
     <row r="22" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A22" s="5">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B22" s="5" t="s">
         <v>57</v>
@@ -2015,7 +3325,7 @@
     </row>
     <row r="23" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A23" s="5">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B23" s="5" t="s">
         <v>58</v>
@@ -2056,7 +3366,7 @@
     </row>
     <row r="24" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A24" s="5">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B24" s="5" t="s">
         <v>59</v>
@@ -2097,7 +3407,7 @@
     </row>
     <row r="25" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A25" s="5">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B25" s="5" t="s">
         <v>60</v>
@@ -2138,7 +3448,7 @@
     </row>
     <row r="26" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A26" s="5">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B26" s="5" t="s">
         <v>61</v>
@@ -2175,10 +3485,402 @@
       </c>
       <c r="M26" s="5" t="s">
         <v>46</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B28" s="7">
+        <v>0</v>
+      </c>
+      <c r="C28" s="7">
+        <v>4</v>
+      </c>
+      <c r="D28" s="7">
+        <f>AVERAGE(D2:D6)</f>
+        <v>0.70329206570861558</v>
+      </c>
+      <c r="E28" s="7">
+        <f>AVERAGE(E2:E6)</f>
+        <v>0.52311198274858794</v>
+      </c>
+      <c r="F28" s="7">
+        <f>AVERAGE(F2:F6)</f>
+        <v>0.50145421213850783</v>
+      </c>
+      <c r="G28" s="7">
+        <f>AVERAGE(G2:G6)</f>
+        <v>0.48680568479667824</v>
+      </c>
+      <c r="H28" s="7">
+        <f>AVERAGE(H2:H6)</f>
+        <v>2517</v>
+      </c>
+      <c r="I28" s="7">
+        <f t="shared" ref="I28:K28" si="0">AVERAGE(I2:I6)</f>
+        <v>0.7139857994580977</v>
+      </c>
+      <c r="J28" s="7">
+        <f>AVERAGE(J2:J6)</f>
+        <v>0.72125218942274305</v>
+      </c>
+      <c r="K28" s="7">
+        <f t="shared" si="0"/>
+        <v>0.70998326626870367</v>
+      </c>
+      <c r="L28" s="7">
+        <f>AVERAGE(L2:L6)</f>
+        <v>2454.4</v>
+      </c>
+      <c r="M28" s="7" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B29" s="2">
+        <v>1</v>
+      </c>
+      <c r="C29" s="2">
+        <v>4</v>
+      </c>
+      <c r="D29" s="2">
+        <f>AVERAGE(D7:D11)</f>
+        <v>0.71669260590504691</v>
+      </c>
+      <c r="E29" s="2">
+        <f t="shared" ref="E29:L29" si="1">AVERAGE(E7:E11)</f>
+        <v>0.52592620707718185</v>
+      </c>
+      <c r="F29" s="2">
+        <f t="shared" si="1"/>
+        <v>0.5017797485497717</v>
+      </c>
+      <c r="G29" s="2">
+        <f t="shared" si="1"/>
+        <v>0.49059497183297041</v>
+      </c>
+      <c r="H29" s="2">
+        <f t="shared" si="1"/>
+        <v>2528</v>
+      </c>
+      <c r="I29" s="2">
+        <f t="shared" si="1"/>
+        <v>0.72386407535312203</v>
+      </c>
+      <c r="J29" s="2">
+        <f t="shared" si="1"/>
+        <v>0.73049347439134571</v>
+      </c>
+      <c r="K29" s="2">
+        <f t="shared" si="1"/>
+        <v>0.71817407645282905</v>
+      </c>
+      <c r="L29" s="2">
+        <f t="shared" si="1"/>
+        <v>2480.4</v>
+      </c>
+      <c r="M29" s="2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B30" s="3">
+        <v>2</v>
+      </c>
+      <c r="C30" s="3">
+        <v>4</v>
+      </c>
+      <c r="D30" s="3">
+        <f>AVERAGE(D12:D16)</f>
+        <v>0.59204270461013797</v>
+      </c>
+      <c r="E30" s="3">
+        <f t="shared" ref="E30:L30" si="2">AVERAGE(E12:E16)</f>
+        <v>0.57884360502790888</v>
+      </c>
+      <c r="F30" s="3">
+        <f t="shared" si="2"/>
+        <v>0.50256460083823262</v>
+      </c>
+      <c r="G30" s="3">
+        <f t="shared" si="2"/>
+        <v>0.49889148104691994</v>
+      </c>
+      <c r="H30" s="3">
+        <f t="shared" si="2"/>
+        <v>1562.6</v>
+      </c>
+      <c r="I30" s="3">
+        <f t="shared" si="2"/>
+        <v>0.60898821490402066</v>
+      </c>
+      <c r="J30" s="3">
+        <f t="shared" si="2"/>
+        <v>0.60478424180737389</v>
+      </c>
+      <c r="K30" s="3">
+        <f t="shared" si="2"/>
+        <v>0.58939676514697903</v>
+      </c>
+      <c r="L30" s="3">
+        <f t="shared" si="2"/>
+        <v>1529.8</v>
+      </c>
+      <c r="M30" s="3" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B31" s="4">
+        <v>4</v>
+      </c>
+      <c r="C31" s="4">
+        <v>4</v>
+      </c>
+      <c r="D31" s="4">
+        <f>AVERAGE(D17:D21)</f>
+        <v>0.4538461538461534</v>
+      </c>
+      <c r="E31" s="4">
+        <f t="shared" ref="E31:L31" si="3">AVERAGE(E17:E21)</f>
+        <v>0.5779830133634476</v>
+      </c>
+      <c r="F31" s="4">
+        <f t="shared" si="3"/>
+        <v>0.53690382081686372</v>
+      </c>
+      <c r="G31" s="4">
+        <f t="shared" si="3"/>
+        <v>0.51559002327325254</v>
+      </c>
+      <c r="H31" s="4">
+        <f t="shared" si="3"/>
+        <v>78</v>
+      </c>
+      <c r="I31" s="4">
+        <f t="shared" si="3"/>
+        <v>0.5779830133634476</v>
+      </c>
+      <c r="J31" s="4">
+        <f t="shared" si="3"/>
+        <v>0.53690382081686372</v>
+      </c>
+      <c r="K31" s="4">
+        <f t="shared" si="3"/>
+        <v>0.51559002327325254</v>
+      </c>
+      <c r="L31" s="4">
+        <f t="shared" si="3"/>
+        <v>66</v>
+      </c>
+      <c r="M31" s="4" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B32" s="5">
+        <v>3</v>
+      </c>
+      <c r="C32" s="5">
+        <v>32</v>
+      </c>
+      <c r="D32" s="5">
+        <f>AVERAGE(D22:D26)</f>
+        <v>0.42172329706607614</v>
+      </c>
+      <c r="E32" s="5">
+        <f>AVERAGE(E22:E26)</f>
+        <v>0.55822577659043782</v>
+      </c>
+      <c r="F32" s="5">
+        <f>AVERAGE(F22:F26)</f>
+        <v>0.61085775284772714</v>
+      </c>
+      <c r="G32" s="5">
+        <f>AVERAGE(G22:G26)</f>
+        <v>0.51773158451892021</v>
+      </c>
+      <c r="H32" s="5">
+        <f>AVERAGE(H22:H26)</f>
+        <v>77.8</v>
+      </c>
+      <c r="I32" s="5">
+        <f>AVERAGE(I22:I26)</f>
+        <v>0.59188025671325439</v>
+      </c>
+      <c r="J32" s="5">
+        <f>AVERAGE(J22:J26)</f>
+        <v>0.53695889623454973</v>
+      </c>
+      <c r="K32" s="5">
+        <f>AVERAGE(K22:K26)</f>
+        <v>0.5043924314176832</v>
+      </c>
+      <c r="L32" s="5">
+        <f>AVERAGE(L22:L26)</f>
+        <v>61.6</v>
+      </c>
+      <c r="M32" s="5" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="34" spans="2:9" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B34" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="C34" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="D34" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="E34" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="F34" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="G34" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="H34" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="I34" s="8" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="35" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B35" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="C35" s="7">
+        <v>0.70329206570861558</v>
+      </c>
+      <c r="D35" s="7">
+        <v>0.52311198274858794</v>
+      </c>
+      <c r="E35" s="7">
+        <v>0.50145421213850783</v>
+      </c>
+      <c r="F35" s="7">
+        <v>0.48680568479667824</v>
+      </c>
+      <c r="G35" s="7">
+        <v>0.7139857994580977</v>
+      </c>
+      <c r="H35" s="7">
+        <v>0.72125218942274305</v>
+      </c>
+      <c r="I35" s="7">
+        <v>0.70998326626870367</v>
+      </c>
+    </row>
+    <row r="36" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B36" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="C36" s="2">
+        <v>0.71669260590504691</v>
+      </c>
+      <c r="D36" s="2">
+        <v>0.52592620707718185</v>
+      </c>
+      <c r="E36" s="2">
+        <v>0.5017797485497717</v>
+      </c>
+      <c r="F36" s="2">
+        <v>0.49059497183297041</v>
+      </c>
+      <c r="G36" s="2">
+        <v>0.72386407535312203</v>
+      </c>
+      <c r="H36" s="2">
+        <v>0.73049347439134571</v>
+      </c>
+      <c r="I36" s="2">
+        <v>0.71817407645282905</v>
+      </c>
+    </row>
+    <row r="37" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B37" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="C37" s="3">
+        <v>0.59204270461013797</v>
+      </c>
+      <c r="D37" s="3">
+        <v>0.57884360502790888</v>
+      </c>
+      <c r="E37" s="3">
+        <v>0.50256460083823262</v>
+      </c>
+      <c r="F37" s="3">
+        <v>0.49889148104691994</v>
+      </c>
+      <c r="G37" s="3">
+        <v>0.60898821490402066</v>
+      </c>
+      <c r="H37" s="3">
+        <v>0.60478424180737389</v>
+      </c>
+      <c r="I37" s="3">
+        <v>0.58939676514697903</v>
+      </c>
+    </row>
+    <row r="38" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B38" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="C38" s="4">
+        <v>0.4538461538461534</v>
+      </c>
+      <c r="D38" s="4">
+        <v>0.5779830133634476</v>
+      </c>
+      <c r="E38" s="4">
+        <v>0.53690382081686372</v>
+      </c>
+      <c r="F38" s="4">
+        <v>0.51559002327325254</v>
+      </c>
+      <c r="G38" s="4">
+        <v>0.5779830133634476</v>
+      </c>
+      <c r="H38" s="4">
+        <v>0.53690382081686372</v>
+      </c>
+      <c r="I38" s="4">
+        <v>0.51559002327325254</v>
+      </c>
+    </row>
+    <row r="39" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B39" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="C39" s="5">
+        <v>0.42172329706607614</v>
+      </c>
+      <c r="D39" s="5">
+        <v>0.55822577659043782</v>
+      </c>
+      <c r="E39" s="5">
+        <v>0.61085775284772714</v>
+      </c>
+      <c r="F39" s="5">
+        <v>0.51773158451892021</v>
+      </c>
+      <c r="G39" s="5">
+        <v>0.59188025671325439</v>
+      </c>
+      <c r="H39" s="5">
+        <v>0.53695889623454973</v>
+      </c>
+      <c r="I39" s="5">
+        <v>0.5043924314176832</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:M1"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>